<commit_message>
another README update / cards.xlsx update
</commit_message>
<xml_diff>
--- a/doompy/files/cards.xlsx
+++ b/doompy/files/cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azabicki/Sync/Projects/DoomPy/doompy/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CE6AC9-2CF3-2446-A79E-BDF8F2823E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30E8CEB-303A-AA41-A675-8B90EFCC747B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="500" windowWidth="36000" windowHeight="20200" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20200" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
   </bookViews>
   <sheets>
     <sheet name="traits" sheetId="1" r:id="rId1"/>
@@ -3263,9 +3263,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AE435C-BBFF-4D4C-B457-AFC1FAEE6491}">
   <dimension ref="A1:Z338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A284" sqref="A284"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4323,7 +4323,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B31" t="s">
         <v>753</v>
@@ -4722,7 +4722,7 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B43" t="s">
         <v>90</v>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B52" t="s">
         <v>743</v>
@@ -5402,7 +5402,7 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B63" t="s">
         <v>744</v>
@@ -7407,7 +7407,7 @@
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B125" t="s">
         <v>763</v>
@@ -7611,7 +7611,7 @@
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B131" t="s">
         <v>745</v>
@@ -8149,7 +8149,7 @@
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B147" t="s">
         <v>747</v>
@@ -8184,7 +8184,7 @@
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B148" t="s">
         <v>748</v>
@@ -8882,7 +8882,7 @@
     </row>
     <row r="168" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B168" t="s">
         <v>749</v>
@@ -9051,7 +9051,7 @@
     </row>
     <row r="173" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B173" t="s">
         <v>764</v>
@@ -9456,7 +9456,7 @@
     </row>
     <row r="185" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B185" t="s">
         <v>755</v>
@@ -11019,7 +11019,7 @@
     </row>
     <row r="232" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B232" t="s">
         <v>750</v>
@@ -11882,7 +11882,7 @@
     </row>
     <row r="258" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B258" t="s">
         <v>757</v>
@@ -12335,7 +12335,7 @@
     </row>
     <row r="271" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B271" t="s">
         <v>751</v>
@@ -12778,7 +12778,7 @@
     </row>
     <row r="284" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B284" t="s">
         <v>752</v>
@@ -13492,7 +13492,7 @@
     </row>
     <row r="305" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B305" t="s">
         <v>756</v>

</xml_diff>

<commit_message>
added second TERROR BEAK
</commit_message>
<xml_diff>
--- a/doompy/files/cards.xlsx
+++ b/doompy/files/cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azabicki/Sync/Projects/DoomPy/doompy/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30E8CEB-303A-AA41-A675-8B90EFCC747B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC735BB4-0B2F-8248-974F-2F3AC07AF1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20200" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
   </bookViews>
@@ -3263,9 +3263,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AE435C-BBFF-4D4C-B457-AFC1FAEE6491}">
   <dimension ref="A1:Z338"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A281" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="E304" sqref="E304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13474,7 +13474,7 @@
         <v>149</v>
       </c>
       <c r="C304">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D304" s="10" t="s">
         <v>1</v>

</xml_diff>